<commit_message>
added test cases 4 star
</commit_message>
<xml_diff>
--- a/ttfd_output_05-12-2025.xlsx
+++ b/ttfd_output_05-12-2025.xlsx
@@ -3,13 +3,81 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+  <sheets>
+    <sheet sheetId="1" name="Demo" state="visible" r:id="rId4"/>
+  </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+  <si>
+    <t>Scenario</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Run Time</t>
+  </si>
+  <si>
+    <t>Time taken to fully drawn (TTFD)</t>
+  </si>
+  <si>
+    <t>24.2s</t>
+  </si>
+  <si>
+    <t>10:44 AM EST</t>
+  </si>
+  <si>
+    <t>State change Arizona to New York</t>
+  </si>
+  <si>
+    <t>2.7s</t>
+  </si>
+  <si>
+    <t>County Change &gt; 1st 2 (Albany and Allegany)</t>
+  </si>
+  <si>
+    <t>2.1s</t>
+  </si>
+  <si>
+    <t>Plan type Change (Local HMO to Local PPO)</t>
+  </si>
+  <si>
+    <t>1.6s</t>
+  </si>
+  <si>
+    <t>SNP Plan Change (DSNP to Non SNP)</t>
+  </si>
+  <si>
+    <t>2.6s</t>
+  </si>
+  <si>
+    <t>Base PLAN Selection (H3418_004 to H3418_008)</t>
+  </si>
+  <si>
+    <t>1.1s</t>
+  </si>
+  <si>
+    <t>Comparison PLan Selection (H2775_105 to H2775_106)</t>
+  </si>
+  <si>
+    <t>0.6s</t>
+  </si>
+  <si>
+    <t>4 stars &amp; up</t>
+  </si>
+  <si>
+    <t>1.0s</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -17,13 +85,21 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD3D3D3"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -38,8 +114,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -375,4 +454,119 @@
   </a:objectDefaults>
   <a:extraClrSchemeLst/>
 </a:theme>
+</file>
+
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C9"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="60" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
 </file>
</xml_diff>